<commit_message>
moved run data into plotting directory
</commit_message>
<xml_diff>
--- a/spreadsheets/run_plan.xlsx
+++ b/spreadsheets/run_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\Dissertation\Parallel-PSO-OPF-Scalability\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2410F9-F337-4939-B385-3BEF98C8380F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72901AC2-D143-4BA8-9784-E517569E4677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="1500" windowWidth="21600" windowHeight="13920" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="serialRuns" sheetId="1" r:id="rId1"/>
@@ -157,9 +157,6 @@
     <t>PSO</t>
   </si>
   <si>
-    <t>Particle Warm Optimization</t>
-  </si>
-  <si>
     <t>OPF</t>
   </si>
   <si>
@@ -194,6 +191,9 @@
   </si>
   <si>
     <t>full form</t>
+  </si>
+  <si>
+    <t>Particle Swarm Optimization</t>
   </si>
 </sst>
 </file>
@@ -8257,16 +8257,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>120015</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>232410</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>598170</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8298,16 +8298,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8372,16 +8372,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8415,16 +8415,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8453,16 +8453,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9103,8 +9103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1102CE02-4A00-4625-A7BD-467D2E2DB84D}">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12455,7 +12455,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12465,42 +12465,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
         <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -12508,15 +12508,15 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>